<commit_message>
1 - simple logic of places
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Лист1!$A$1:$G$261</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Лист1!$A$1:$G$292</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="1082">
   <si>
     <t>id</t>
   </si>
@@ -2788,9 +2788,6 @@
     <t>Центральная районная библиотека им. В. Г. Короленко, входящая в состав МКУК «Централизованная библиотечная система» Нижегородского района, является одной из старейших библиотек Нижнего Новгорода и располагается по адресу улица Родионова, 199, к.2; её история начинается в конце XIX века, а с 1921 года библиотека носит имя писателя и гуманиста В. Г. Короленко, что подчёркивает её культурное и образовательное значение. Сегодня это современное и уютное книжное пространство, постоянно привлекающее нижегородцев всех возрастов, где в просторных залах регулярно проводятся конференции, фестивали, праздничные программы, встречи с писателями, поэтами и известными деятелями культуры, театрализованные представления, мастер-классы и образовательные семинары. Библиотека оснащена современным аудио- и видеооборудованием, 3D-принтером, голографическими проекторами и другими техническими средствами, что позволяет реализовывать широкий спектр интерактивных мероприятий и образовательных проектов, выходящих за рамки традиционной библиотечной деятельности. Кроме того, библиотека активно участвует в грантовых проектах, направленных на учёт особенностей территории, интересов целевой аудитории и социальных и культурных факторов, благодаря чему создаются уникальные программы и инициативы, ориентированные на изучение и сохранение культурного наследия, развитие творческих способностей и формирование навыков критического мышления. Посетители могут не только пользоваться богатым фондом литературы и периодики, но и участвовать в творческих лабораториях, образовательных курсах, клубах по интересам, практических занятиях и выставках, что делает библиотеку интересной для школьников, студентов, педагогов, исследователей, семей с детьми и всех, кто стремится к культурному обогащению, образовательному росту и активному участию в жизни городской общины.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Детская библиотека — филиал №5 им. Н.Ф. Гастелло, расположенная по адресу проспект Героев, дом 12 в Московском районе Нижнего Новгорода, является одной из старейших детских библиотек города, открытой в 1952 году и изначально носившей название «Детская библиотека №2 Сталинского района», что отражает её многолетнюю историю и важность в культурной жизни района; библиотека занимает первый этаж трёхэтажного жилого дома и за годы существования стала уютным и нарядным центром притяжения детей с окрестных улиц, предлагая им обширный фонд литературы для младшего и старшего возраста, читальный зал для работы и изучения книг, а также регулярные интерактивные мероприятия, конкурсы, викторины, мастер-классы и тематические акции, в которых активно участвуют школьники и педагоги из соседней школы №64; сотрудники библиотеки создают программы, направленные на развитие навыков вдумчивого чтения, творческого мышления и интереса к литературе, проводят встречи с авторами и творческие лаборатории, организуют книжные выставки, посвящённые актуальным темам, а также предоставляют современные услуги для посетителей, включая ксерокопирование и распечатку материалов с электронных носителей; библиотека уникальна тем, что сочетает традиционные библиотечные функции с активным вовлечением детей в культурную и образовательную жизнь города, она интересна для младших школьников, подростков, педагогов, родителей, а также всех, кто стремится познакомить детей с литературой, развить их творческий потенциал и приобщить к библиотечной культуре, делая её важной площадкой для социализации и образовательного роста в Московском районе Нижнего Новгорода.</t>
   </si>
   <si>
@@ -3002,13 +2999,346 @@
   </si>
   <si>
     <t>Мозаика «Плодородие» находится в Нижнем Новгороде по адресу ул. Юлиуса Фучика, д.23А и была создана в 1982 году автором, имя которого не установлено. Эта композиция посвящена теме сельского хозяйства, изобилия и плодородия земли, символизируя труд человека, гармонию с природой и процветание общества. Мозаика выполнена в характерной для советской монументально-декоративной школы манере, с использованием керамических элементов, что позволяет передать яркость цветов, фактурность и выразительность образов. Объект уникален своей тематикой и художественным решением, расположение на фасаде здания делает его доступным для широкой аудитории, включая жителей района, туристов и студентов, позволяя наблюдать детали и смысловую нагрузку работы. Мозаика входит в реестр произведений советского монументально-декоративного искусства Нижегородской области, что подчеркивает её историческую, художественную и культурную значимость и делает её интересной для исследователей советского искусства, студентов художественных специальностей, краеведов, туристов и всех, кто ценит наследие монументального искусства советского периода.</t>
+  </si>
+  <si>
+    <t>Ресторан "Митрич"</t>
+  </si>
+  <si>
+    <t>Это стейк-хаус премиум-класса, известный своей атмосферой и качественным обслуживанием. В меню представлены разнообразные стейки, морепродукты, а также блюда европейской кухни. Средний чек составляет около 2000–3000 рублей. Гости отмечают высокий уровень сервиса и вкусную еду. Более подробную информацию можно найти на официальном сайте ресторана: mitrichsteakhouse.ru</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Ковалихинская, 8</t>
+  </si>
+  <si>
+    <t>Ресторан "Escape"</t>
+  </si>
+  <si>
+    <t>Ресторан «Café 38»</t>
+  </si>
+  <si>
+    <t>Это ресторан с европейской, русской и авторской кухней, предлагающий разнообразные блюда и напитки. Средний чек составляет около 1500 рублей. Заведение известно своим качественным обслуживанием и вкусной едой. Подробнее о ресторане можно узнать на сайте: novgorod.ugosti.com</t>
+  </si>
+  <si>
+    <t>Ресторан «LE GRILL»</t>
+  </si>
+  <si>
+    <t>г. Нижний Новгород, ул. Белинского, 11/66</t>
+  </si>
+  <si>
+    <t>POINT(56.310357 44.000291)</t>
+  </si>
+  <si>
+    <t>Представляет собой стильный современный гриль-ресторан с тремя просторными залами в центре города, рядом с парком Пушкина, интерьер оформлен в стиле фьюжн с открытой кухней, основная кухня – авторская и европейская с акцентом на мясные блюда, над угольной печью Josper готовят мраморную говядину зернового откорма с сохранением сочности и вкусовых качеств, средний чек в ресторане колеблется примерно от 1500 до 2500 рублей, отзывы отмечают высокий уровень подачи и гостеприимство, сайт legrill.ru.</t>
+  </si>
+  <si>
+    <t>Ресторан «Pitnica»</t>
+  </si>
+  <si>
+    <t>г. Нижний Новгород, ул. Большая Покровская, д. 25</t>
+  </si>
+  <si>
+    <t>Современный ресторан-пивоварня с чешско-европейской кухней: меню включает сет гриль-колбасок, плескавицу, штрудель, сезонное пиво на кранах; средний чек около 1300 ₽; отзывы отмечают атмосферу, живую музыку и хорошее обслуживание; сайт: http://nn.pitnica.ru/</t>
+  </si>
+  <si>
+    <t>г. Нижний Новгород, ул. Большая Покровская, д. 46</t>
+  </si>
+  <si>
+    <t>Это итальянское семейное кафе с просторным залом, предлагающее пасту, пиццу, десерты и бизнес-ланчи; средний чек примерно 1100–1500 ₽; отзывы указывают на отличную атмосферу и удобное расположение; сайт: biblioteca-nn.ru</t>
+  </si>
+  <si>
+    <t>POINT(56.326800 44.008500)</t>
+  </si>
+  <si>
+    <t>Кафе-ресторан «Biblioteca»</t>
+  </si>
+  <si>
+    <t>г. Нижний Новгород, ул. Октябрьская, д. 9А</t>
+  </si>
+  <si>
+    <t>POINT(56.328000 44.007200)</t>
+  </si>
+  <si>
+    <t>Современное кафе-формат с бургер-меню (классические и вегетарианские варианты), напитками и атмосферой для отдыха; средний чек ~800–1200 ₽; отзывы отмечают демократичность и хорошую локацию; сайт: salut-nn.ru</t>
+  </si>
+  <si>
+    <t>Кафе «Salut»</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Коминтерна 172</t>
+  </si>
+  <si>
+    <t>POINT(56.323000 44.000000)</t>
+  </si>
+  <si>
+    <t>Небольшое кафе-пекарня с историей, специализирующееся на пирожках и традиционной советской кухне, популярное среди местных жителей; кухня — русская, европейская и восточная с акцентом на выпечку; средний чек ~300-600 ₽; отзывы отмечают свежую выпечку, доброжелательное обслуживание и атмосферу «как дома»</t>
+  </si>
+  <si>
+    <t>Кафе «Сормовская пирожковая»</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Ковалихинская, д. 8</t>
+  </si>
+  <si>
+    <t>POINT(56.323333 44.011457)</t>
+  </si>
+  <si>
+    <t>Это премиальный стейк-хаус в центре города от проекта «Еда и Культура», расположенный на втором этаже современного бизнес-центра и известный своей камерной атмосферой с открытой кухней и акцентом на выдержанное мраморное мясо и гриль; кухня — авторская европейская со спецфокусом на стейках (рибай, томагавк, шот-реб), выдержанных стейках разных прожарок, тартаре, морепродуктах, сезонных гарнирах и авторских соусах; в меню представлены разнообразные позиции от закусок (карпаччо, цезарь с говядиной) до основных блюд (стейки USDA/Angus, лобстер, рыба на гриле) и десертов; средний чек ориентировочно 2000–3000 ₽ в зависимости от выбора мяса и вина; отзывы на Яндекс/TripAdvisor и локальных ресурсах в целом очень положительные, посетители отмечают высокое качество стейков, профессиональный сервис и атмосферу, но указывают на цену как на главный минус; официальный сайт: https://mitrichsteakhouse.ru/</t>
+  </si>
+  <si>
+    <t>Mitrich Steakhouse</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, Октябрьская площадь, д. 1 (КЗ «Юпитер»)</t>
+  </si>
+  <si>
+    <t>POINT(56.323123 44.009077)</t>
+  </si>
+  <si>
+    <t>Семейный ресторан в формате эко-лофт от Novikov Group, известный своей фермерской эстетикой и собственным подходом к сырам и продуктам, просторными залами и сезонной террасой — хорош для семейных ужинов и праздников; кухня — деревенская/итальянско-европейская с упором на фермерские продукты и сырные позиции: домашние закуски, салаты с авторскими заправками, супы, пасты, ризотто, блюда из сезонных овощей, авторские мясные блюда и обширный десертный раздел; в меню есть фирменные сырные тарелки, пасты, стейки, сезонные супы, фирменные десерты; средний чек около 1500 ₽; отзывы равномерно положительные — хвалят интерьер, качество ингредиентов и семейную подачу, некоторые замечают стоимость как выше среднего; официальный сайт: https://syrovarnya.com/syrovarnya-nizhnij-novgorod</t>
+  </si>
+  <si>
+    <t>Ресторан "Сыроварня (Syrovarnya)"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Рождественская, д. 30</t>
+  </si>
+  <si>
+    <t>POINT(56.327655 43.986197)</t>
+  </si>
+  <si>
+    <t>Ресторан современной русской кухни, расположенный в одном из старинных купеческих особняков, где интерьер и историческая архитектура соседствуют с авторской подачей и тщательным выбором локальных продуктов; кухня — современная русская с элементами «new nordic» и авторских техник: в меню — сезонные закуски, холодные и горячие закуски из локальной рыбы и мяса, авторские супы, блюда из дикой рыбы, мясные композиции, десерты с ферментированными и лесными ингредиентами; меню меняется по сезону, типичные позиции: тартар из говядины, уха/супы из местной рыбы, рифленые гарниры, десерты с лесными ягодами и авторскими кремами; средний чек примерно 1500–2500 ₽; отзывы на 2GIS/TripAdvisor отмечают высокий уровень кухни, креативность шефа и атмосферу, ресторан рассматривают как место для особых случаев; сайт: http://yalerestaurant.ru/</t>
+  </si>
+  <si>
+    <t>Ресторан "YALE"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Рождественская, д. 39</t>
+  </si>
+  <si>
+    <t>POINT(56.327980 43.985738)</t>
+  </si>
+  <si>
+    <t>Итальянская траттория/ресторан, входящая в число известных гастрономических адресов города, предлагает традиционную итальянскую кухню в современной интерпретации — уютный зал, открытая кухня и внимание к ингредиентам; кухня — итальянская (пицца на дровах, домашняя паста, антипасти, морепродукты, классические тирамису и джелато); в меню: ассорти антипасти, тапас-плато, свежая пицца, сезонные пасты, морепродукты, салаты и авторские десерты; средний чек порядка 1000–1500 ₽; отзывы пользователей отмечают отличную пиццу и пасту, корректное соотношение цены и качества и удобное расположение на пешеходной улице; сайт: https://pinci.ru/</t>
+  </si>
+  <si>
+    <t>Ресторан "Pinci"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, Верхне-Волжская набережная, д. 8</t>
+  </si>
+  <si>
+    <t>POINT(56.329168 44.018644)</t>
+  </si>
+  <si>
+    <t>Крупное ресторанное пространство на набережной с видом на Волгу, совмещающее ресторан морепродуктов/европейской кухни и азиатскую ветку Escape Asia, популярное благодаря летней веранде, панорамам и вечерним мероприятиям; кухня — морепродукты и авторская паназиатская/европейская кухня: в меню представлены устрицы, севиче, разнообразные блюда из рыбы и морепродуктов, суши/сеты в зоне Asia, а также фирменные коктейли и десерты; средний чек ориентировочно 1500–2500 ₽ в зависимости от выбора морепродуктов и напитков; отзывы на 2GIS/TripAdvisor/Yandex отмечают локацию у воды, свежесть морепродуктов и праздник атмосферы вечером, иногда критикуют сервис в пиковые часы; сайт: https://escape.rest/</t>
+  </si>
+  <si>
+    <t>Ресторан «Хачапури и Вино»</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Коминтерна, д. 164</t>
+  </si>
+  <si>
+    <t>Уютный грузинский ресторан, оформленный в теплых тонах с элементами национального декора, где можно насладиться традиционной кухней Грузии и атмосферой гостеприимства. Кухня — грузинская с упором на домашние блюда, приготовленные по классическим рецептам: хачапури всех видов (по-аджарски, по-имеретински, мегрельский), хинкали, чахохбили, оджахури, шашлыки и ароматные соусы. Меню дополнено подборкой грузинских вин и десертов, включая чурчхелу и пахлаву. Средний чек составляет 1000–1500 ₽. Отзывы гостей отмечают большие порции, подлинный вкус блюд и приветливое обслуживание, а также семейную атмосферу, идеально подходящую для ужинов и праздников. Официальный сайт: https://hivino.ru/</t>
+  </si>
+  <si>
+    <t>POINT(56.349278 43.862944)</t>
+  </si>
+  <si>
+    <t>POINT(44.011457 56.323333)</t>
+  </si>
+  <si>
+    <t>POINT(43.982891 56.326777)</t>
+  </si>
+  <si>
+    <t>POINT(43.999042 56.321172)</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Рождественская, 38</t>
+  </si>
+  <si>
+    <t>Skuratov Coffee</t>
+  </si>
+  <si>
+    <t>POINT(56.3295 43.9930)</t>
+  </si>
+  <si>
+    <t>Кафе‑кофейня с акцентом на здоровое питание: десерты без сахара, чизкейки, кофе, напитки; средний чек около ~500 ₽. Подходит как для десерта после прогулки, так и для лёгкого завтрака. Рейтинг ~4.5.</t>
+  </si>
+  <si>
+    <t>Современная спешелти‑кофейня с собственной обжаркой кофе и лабораторным подходом: здесь предлагают эспрессо, фильтр‑кофе, аэропресс и даже газированный нитро‑кофе, наряду с завтраками и легкими закусками. Меню включает завтраки с круассаном с миндальным кремом (~260 ₽), боулы с киноа (~290 ₽) и профес-баристами; средний чек без напитков около ~400 ₽. Заведение получает высокие отзывы за атмосферу, качество напитков и скорость обслуживания (рейтинг ~4.8–5.0). Сайт: skuratovcoffee.ru</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Большая Покровская, 60</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Костина, 3</t>
+  </si>
+  <si>
+    <t>POINT(56.3000 43.9850)</t>
+  </si>
+  <si>
+    <t>Уютная кофейня‑бар, ориентированная на фильтр‑кофе, авторские напитки и десерты ручной работы, подходит для неспешного кофе с друзьями или работы. Средний чек около ~350‑400 ₽; рейтинг ~4.9. Посетители отмечают внимательность бариста и атмосферу.</t>
+  </si>
+  <si>
+    <t>POINT(56.3275 44.0090)</t>
+  </si>
+  <si>
+    <t>Кондитерская ПП №1</t>
+  </si>
+  <si>
+    <t>Чёрточка</t>
+  </si>
+  <si>
+    <t>«Бенье»</t>
+  </si>
+  <si>
+    <t>Нижний Новогород, ул. Большая Покровская, 20</t>
+  </si>
+  <si>
+    <t>POINT(56.3236 44.0008)</t>
+  </si>
+  <si>
+    <t>«Мистер Бублик»</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Невзоровых, 85</t>
+  </si>
+  <si>
+    <t>POINT(56.3090 44.0525)</t>
+  </si>
+  <si>
+    <t>Заведение представляет собой уютную кондитерскую‑пекарню с большим выбором авторских десертов, пирожных и тортов на заказ, а также завтраков и кофе‑брейков; кухня — европейская, с акцентом на сладкое и кофе, меню включает муссовые торты (например, «малина‑личи», «шоколад‑малина» по ~450‑500 ₽ за порцию 120 г), слойки, эклеры от ~260 ₽, торты на заказ от ~2800₽/кг; средний чек около 400‑600 ₽; отзывы отмечают высокое качество десертов и уютную атмосферу (рейтинг ~4.4‑4.8); сайт: mrbublik.ru.</t>
+  </si>
+  <si>
+    <t>Бистро‑пекарня с французским акцентом: меню включает круассаны с начинками, десертные тарталетки, эклеры, кофе‑спешелти; кухня — европейская кондитерская; средний чек ~350‑500₽; рейтинг ~4.8 при ~1700 отзывах, отзывы подчёркивают высокое качество выпечки и комфортную атмосферу. Сайт: benye‑nn.ru.</t>
+  </si>
+  <si>
+    <t>Стильная студия‑кондитерская с акцентом на торты и десерты ручной работы: в меню представлены торты на заказ (кремовые, ягодные, 3D‑формы), капкейки, пирожные и зефир, все из натуральных ингредиентов; средний чек ~700‑1200 ₽ за десерт порционного формата, торты от ~800 ₽/кг; отзывы отмечают оригинальность вкусовых сочетаний и индивидуальный подход; сайт: https://ilgusto‑nn.ru</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Богородского, д. 7/2</t>
+  </si>
+  <si>
+    <t>POINT(56.3164 44.0449)</t>
+  </si>
+  <si>
+    <t>Домашняя кондитерская «il gusto»</t>
+  </si>
+  <si>
+    <t>Нижний Новогород, ул. Большая Покровская, 2/1</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Большая Печёрская, д. 44</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Ковалихинская, д. 4А</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, Верхне‑Волжская набережная, д. 2А</t>
+  </si>
+  <si>
+    <t>POINT(56.323333 44.032002)</t>
+  </si>
+  <si>
+    <t>POINT(56.329812 44.003485)</t>
+  </si>
+  <si>
+    <t>POINT(56.326100 44.009200)</t>
+  </si>
+  <si>
+    <t>POINT(56.329392 44.011367)</t>
+  </si>
+  <si>
+    <t>Ресторан Pasters</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Большая Покровская, д. 21/5</t>
+  </si>
+  <si>
+    <t>POINT(56.328500 44.003000)</t>
+  </si>
+  <si>
+    <t>Современный итальянский ресторан с минималистичным лофтовым интерьером на одной из главных пешеходных улиц города, идеально подходит для ужинов с друзьями и романтических встреч; кухня — европейская с акцентом на итальянскую: пасты, ризотто, свежая рыба или мясо на гриле, десерты, авторские коктейли; меню включает фирменные пасты («тальятелле с трюфелем»), ризотто с морепродуктами, десертные тарты, винная карта с итальянскими и французскими винами; средний чек около 2200 ₽; отзывы отмечают качество блюд, стильный интерьер и высокий уровень обслуживания; официальный сайт: https://berezkagroup.ru/</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Большая Покровская, д. 4</t>
+  </si>
+  <si>
+    <t>POINT(56.329200 44.001800)</t>
+  </si>
+  <si>
+    <t>Уютный ресторан с русской и нижегородской кухней, где гости могут ощутить колорит старой Руси в интерьере с тематическими залами и деревянными деталями; кухня — русская/европейская с акцентом на утку и традиционные блюда: борщ с уткой, ножка утки конфи, каша из топора, салаты с раковыми шейками; меню также включает сезонные блюда, закуски и десерты; средний чек около 2000 ₽ без напитков; отзывы подчеркивают большие порции, аромат блюд и тематическую атмосферу; официальный сайт: https://samovardautki.ru/</t>
+  </si>
+  <si>
+    <t>Ресторан "Самовар да Утки"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Октябрьская, д. 9Б</t>
+  </si>
+  <si>
+    <t>POINT(56.330000 44.000000)</t>
+  </si>
+  <si>
+    <t>Пиццерия в центре города, специализирующаяся на неаполитанской пицце, приготовленной в дровяной печи, с уютным интерьером и винным баром; кухня — итальянская (пицца на дровах) с дополнением европейских блюд: паста, салаты, десерты, а также авторские сочетания пиццы с топпингами (например, груша‑горгонзола, аргентинские креветки); меню включает классические пиццы (Маргарита, Пепперони), авторские пиццы, пасту, салаты, десерты; средний чек ориентировочно 800‑1000 ₽, иногда до 2000 ₽ для вечернего ужина без напитков; отзывы отмечают свежую и сочную пиццу, приятную атмосферу и вежливый сервис; сайт: https://www.facebook.com/yulapizza/</t>
+  </si>
+  <si>
+    <t>Ресторан‑бистро с концепцией все‑дня завтраков, переводящей идею утреннего меню в вечернее гастрономическое время, расположен в историческом здании конца XIX века и предлагает стильный интерьер и атмосферу; кухня — европейская с элементами русской и французской: утренние завтраки, бранчи, а вечером — салаты, супы, стейк‑лосось, десерты; меню включает ватрушки и круассаны, яйца Бенедикт, каши, сеты завтраков, вечернее меню: луковый суп, стейк из лосося, клубничный десерт; средний чек около 1500 ₽ без напитков; отзывы оценивают ресторан на 4.9 и выше, отмечая оригинальность концепции и качество.</t>
+  </si>
+  <si>
+    <t>Ресторан "Министерство Завтраков"</t>
+  </si>
+  <si>
+    <t>Ресторан "Юла Пицца"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, проспект Молодёжный, д. 4А</t>
+  </si>
+  <si>
+    <t>POINT(56.306000 44.058000)</t>
+  </si>
+  <si>
+    <t>Семейный ресторан‑бар с европейской, азиатской и русской кухней, просторными залами, зонами для банкетов и детской комнатой, удобен для семейных мероприятий или встреч групп друзей; кухня — мультикультурная: европейские блюда, азиатские роллы и вок‑блюда, русские классические позиции; меню включает роллы, бургеры, жареный сыр, тартар из говядины, скандинавские бутерброды, салаты и коктейли; средний чек около 700‑2500 ₽ в зависимости от состава компании и напитков; отзывы называют ресторан универсальным для разных форматов и отмечают хорошую кухню; официальный сайт: https://soyuz-rest.ru/</t>
+  </si>
+  <si>
+    <t>Ресторан "Союз"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Родионова, д. 187, ТРЦ «Фантастика»</t>
+  </si>
+  <si>
+    <t>POINT(56.341200 43.999500)</t>
+  </si>
+  <si>
+    <t>Это уютный семейный ресторан с итальянской кухней, который делает акцент на собственном производстве пасты из твердых сортов пшеницы, колбасок и десертов, оформлен в стиле «домашней Италии» с просторным залом, подходит и для семейного ужина, и для встречи с друзьями; кухня — итальянская/европейская: в меню представлены пицца с тонким тестом, паста, домашняя колбаска гриль, утка по‑пекински (хотя не традиционно итальянское блюдо, но есть как фирменная композиция), десерты собственного производства и богатая винная карта; средний чек примерно 1500 ₽ без напитков, ланч‑меню от ~500 ₽; отзывы пользователей дают рейтинг около 4.6‑4.7 из 5, гости отмечают свежесть продуктов, тонкое тесто пиццы, высокое качество десертов, внимательный персонал и семейную атмосферу, некоторые отмечают, что порции могли бы быть чуть больше; сайт: https://www.fantastika-nn.ru/eda/restoran-domashnyaya-italiya</t>
+  </si>
+  <si>
+    <t>Ресторан "Домашняя Италия"</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, Казанское шоссе, д. 11 (ТРК «Индиго Life»)</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, ул. Бетанкура, д. 1 (ТРЦ «Седьмое Небо»)</t>
+  </si>
+  <si>
+    <t>POINT(56.316247 43.965110)</t>
+  </si>
+  <si>
+    <t>Нижний Новгород, пл. Советская, д. 5 (ТРЦ «Жар‑Птица»)</t>
+  </si>
+  <si>
+    <t>POINT(56.329130 43.999200)</t>
+  </si>
+  <si>
+    <t>POINT(56.323573 44.010892)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3029,6 +3359,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0F1115"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -3058,10 +3397,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3073,18 +3413,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3099,7 +3436,12 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3145,16 +3487,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="cultural_sites_202509191434" displayName="cultural_sites_202509191434" ref="A1:G261" tableType="queryTable" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:G261"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="cultural_sites_202509191434" displayName="cultural_sites_202509191434" ref="A1:G292" tableType="queryTable" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:G292"/>
   <tableColumns count="7">
-    <tableColumn id="1" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="0"/>
-    <tableColumn id="2" uniqueName="2" name="address" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" uniqueName="3" name="coordinate" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" uniqueName="4" name="description" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="6" uniqueName="6" name="title" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="1" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" uniqueName="2" name="address" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" uniqueName="3" name="coordinate" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" uniqueName="4" name="description" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="6" uniqueName="6" name="title" queryTableFieldId="6" dataDxfId="1"/>
     <tableColumn id="7" uniqueName="7" name="category_id" queryTableFieldId="7"/>
-    <tableColumn id="8" uniqueName="8" name="url" queryTableFieldId="8" dataDxfId="2"/>
+    <tableColumn id="8" uniqueName="8" name="url" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3423,10 +3765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G261"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A261"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="I288" sqref="I288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6256,7 +6598,7 @@
         <v>350</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>351</v>
@@ -6279,7 +6621,7 @@
         <v>353</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>354</v>
@@ -6302,7 +6644,7 @@
         <v>356</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>357</v>
@@ -6325,7 +6667,7 @@
         <v>359</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>360</v>
@@ -6348,7 +6690,7 @@
         <v>362</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>363</v>
@@ -6371,7 +6713,7 @@
         <v>365</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>366</v>
@@ -6394,7 +6736,7 @@
         <v>368</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>369</v>
@@ -6417,7 +6759,7 @@
         <v>371</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>372</v>
@@ -6440,7 +6782,7 @@
         <v>374</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>375</v>
@@ -6463,7 +6805,7 @@
         <v>159</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>376</v>
@@ -6486,7 +6828,7 @@
         <v>159</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>377</v>
@@ -6509,7 +6851,7 @@
         <v>379</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>380</v>
@@ -6532,7 +6874,7 @@
         <v>382</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>383</v>
@@ -6555,7 +6897,7 @@
         <v>385</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>386</v>
@@ -6578,7 +6920,7 @@
         <v>385</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>387</v>
@@ -6601,7 +6943,7 @@
         <v>389</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>390</v>
@@ -6624,7 +6966,7 @@
         <v>392</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>393</v>
@@ -6647,7 +6989,7 @@
         <v>395</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>396</v>
@@ -6670,7 +7012,7 @@
         <v>398</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>399</v>
@@ -6693,7 +7035,7 @@
         <v>337</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>400</v>
@@ -6854,7 +7196,7 @@
         <v>419</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>420</v>
@@ -6877,7 +7219,7 @@
         <v>293</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>421</v>
@@ -6900,7 +7242,7 @@
         <v>253</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>422</v>
@@ -6923,7 +7265,7 @@
         <v>308</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>424</v>
@@ -6946,7 +7288,7 @@
         <v>426</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>427</v>
@@ -6969,7 +7311,7 @@
         <v>429</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>430</v>
@@ -6992,7 +7334,7 @@
         <v>432</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>433</v>
@@ -7153,7 +7495,7 @@
         <v>451</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>452</v>
@@ -7245,7 +7587,7 @@
         <v>462</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>463</v>
@@ -7429,7 +7771,7 @@
         <v>484</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>485</v>
@@ -7452,7 +7794,7 @@
         <v>486</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>487</v>
@@ -7475,7 +7817,7 @@
         <v>489</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>490</v>
@@ -7636,7 +7978,7 @@
         <v>509</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>510</v>
@@ -7682,7 +8024,7 @@
         <v>491</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>514</v>
@@ -7728,7 +8070,7 @@
         <v>33</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>518</v>
@@ -7820,7 +8162,7 @@
         <v>135</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>527</v>
@@ -7889,7 +8231,7 @@
         <v>535</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>536</v>
@@ -7912,7 +8254,7 @@
         <v>538</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>539</v>
@@ -8004,7 +8346,7 @@
         <v>315</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>549</v>
@@ -8096,7 +8438,7 @@
         <v>57</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>559</v>
@@ -8119,7 +8461,7 @@
         <v>311</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>561</v>
@@ -8142,7 +8484,7 @@
         <v>563</v>
       </c>
       <c r="D205" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>564</v>
@@ -8165,7 +8507,7 @@
         <v>566</v>
       </c>
       <c r="D206" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>567</v>
@@ -8188,7 +8530,7 @@
         <v>569</v>
       </c>
       <c r="D207" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>570</v>
@@ -8257,7 +8599,7 @@
         <v>578</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>579</v>
@@ -8556,7 +8898,7 @@
         <v>287</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="E223" s="1" t="s">
         <v>613</v>
@@ -8625,7 +8967,7 @@
         <v>326</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>620</v>
@@ -8901,7 +9243,7 @@
         <v>655</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E238" s="1" t="s">
         <v>656</v>
@@ -8924,7 +9266,7 @@
         <v>658</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E239" s="1" t="s">
         <v>659</v>
@@ -8947,7 +9289,7 @@
         <v>661</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E240" s="1" t="s">
         <v>662</v>
@@ -8970,7 +9312,7 @@
         <v>664</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E241" s="1" t="s">
         <v>665</v>
@@ -8993,7 +9335,7 @@
         <v>667</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E242" s="1" t="s">
         <v>668</v>
@@ -9016,7 +9358,7 @@
         <v>670</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>671</v>
@@ -9039,7 +9381,7 @@
         <v>673</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E244" s="1" t="s">
         <v>674</v>
@@ -9062,7 +9404,7 @@
         <v>676</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E245" s="1" t="s">
         <v>677</v>
@@ -9085,7 +9427,7 @@
         <v>679</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E246" s="1" t="s">
         <v>680</v>
@@ -9108,7 +9450,7 @@
         <v>682</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E247" s="1" t="s">
         <v>683</v>
@@ -9131,7 +9473,7 @@
         <v>685</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E248" s="1" t="s">
         <v>686</v>
@@ -9154,7 +9496,7 @@
         <v>688</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="E249" s="1" t="s">
         <v>689</v>
@@ -9177,7 +9519,7 @@
         <v>691</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>692</v>
@@ -9200,7 +9542,7 @@
         <v>694</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>695</v>
@@ -9223,7 +9565,7 @@
         <v>697</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E252" s="1" t="s">
         <v>698</v>
@@ -9246,7 +9588,7 @@
         <v>700</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E253" s="1" t="s">
         <v>701</v>
@@ -9269,7 +9611,7 @@
         <v>703</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E254" s="1" t="s">
         <v>704</v>
@@ -9292,7 +9634,7 @@
         <v>706</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>707</v>
@@ -9315,7 +9657,7 @@
         <v>392</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E256" s="1" t="s">
         <v>709</v>
@@ -9338,7 +9680,7 @@
         <v>711</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E257" s="1" t="s">
         <v>712</v>
@@ -9361,7 +9703,7 @@
         <v>714</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E258" s="1" t="s">
         <v>715</v>
@@ -9384,7 +9726,7 @@
         <v>717</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E259" s="1" t="s">
         <v>718</v>
@@ -9407,7 +9749,7 @@
         <v>39</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E260" s="1" t="s">
         <v>719</v>
@@ -9426,11 +9768,11 @@
       <c r="B261" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="C261" s="5" t="s">
-        <v>900</v>
+      <c r="C261" t="s">
+        <v>1031</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E261" s="5" t="s">
         <v>721</v>
@@ -9440,11 +9782,667 @@
       </c>
       <c r="G261" s="1"/>
     </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A262" s="7">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>973</v>
+      </c>
+      <c r="C262" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D262" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="F262">
+        <v>11</v>
+      </c>
+      <c r="G262" s="1"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A263" s="7">
+        <v>263</v>
+      </c>
+      <c r="B263" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C263" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D263" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="F263">
+        <v>11</v>
+      </c>
+      <c r="G263" s="1"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A264" s="7">
+        <v>264</v>
+      </c>
+      <c r="B264" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C264" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D264" t="s">
+        <v>976</v>
+      </c>
+      <c r="E264" t="s">
+        <v>975</v>
+      </c>
+      <c r="F264">
+        <v>11</v>
+      </c>
+      <c r="G264" s="1"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A265" s="7">
+        <v>265</v>
+      </c>
+      <c r="B265" t="s">
+        <v>978</v>
+      </c>
+      <c r="C265" t="s">
+        <v>979</v>
+      </c>
+      <c r="D265" t="s">
+        <v>980</v>
+      </c>
+      <c r="E265" t="s">
+        <v>977</v>
+      </c>
+      <c r="F265">
+        <v>11</v>
+      </c>
+      <c r="G265" s="1"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A266" s="7">
+        <v>266</v>
+      </c>
+      <c r="B266" t="s">
+        <v>982</v>
+      </c>
+      <c r="C266" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D266" t="s">
+        <v>983</v>
+      </c>
+      <c r="E266" t="s">
+        <v>981</v>
+      </c>
+      <c r="F266">
+        <v>11</v>
+      </c>
+      <c r="G266" s="1"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A267" s="7">
+        <v>267</v>
+      </c>
+      <c r="B267" t="s">
+        <v>984</v>
+      </c>
+      <c r="C267" t="s">
+        <v>986</v>
+      </c>
+      <c r="D267" t="s">
+        <v>985</v>
+      </c>
+      <c r="E267" t="s">
+        <v>987</v>
+      </c>
+      <c r="F267">
+        <v>11</v>
+      </c>
+      <c r="G267" s="1"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A268" s="7">
+        <v>268</v>
+      </c>
+      <c r="B268" t="s">
+        <v>988</v>
+      </c>
+      <c r="C268" t="s">
+        <v>989</v>
+      </c>
+      <c r="D268" t="s">
+        <v>990</v>
+      </c>
+      <c r="E268" t="s">
+        <v>991</v>
+      </c>
+      <c r="F268">
+        <v>11</v>
+      </c>
+      <c r="G268" s="1"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A269" s="7">
+        <v>269</v>
+      </c>
+      <c r="B269" t="s">
+        <v>992</v>
+      </c>
+      <c r="C269" t="s">
+        <v>993</v>
+      </c>
+      <c r="D269" t="s">
+        <v>994</v>
+      </c>
+      <c r="E269" t="s">
+        <v>995</v>
+      </c>
+      <c r="F269">
+        <v>11</v>
+      </c>
+      <c r="G269" s="1"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A270" s="7">
+        <v>270</v>
+      </c>
+      <c r="B270" t="s">
+        <v>996</v>
+      </c>
+      <c r="C270" t="s">
+        <v>997</v>
+      </c>
+      <c r="D270" t="s">
+        <v>998</v>
+      </c>
+      <c r="E270" t="s">
+        <v>999</v>
+      </c>
+      <c r="F270">
+        <v>11</v>
+      </c>
+      <c r="G270" s="1"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A271" s="7">
+        <v>271</v>
+      </c>
+      <c r="B271" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D271" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F271">
+        <v>11</v>
+      </c>
+      <c r="G271" s="1"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A272" s="7">
+        <v>272</v>
+      </c>
+      <c r="B272" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D272" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F272">
+        <v>11</v>
+      </c>
+      <c r="G272" s="1"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A273" s="7">
+        <v>273</v>
+      </c>
+      <c r="B273" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D273" s="9" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F273">
+        <v>11</v>
+      </c>
+      <c r="G273" s="1"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A274" s="7">
+        <v>274</v>
+      </c>
+      <c r="B274" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D274" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E274" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F274">
+        <v>11</v>
+      </c>
+      <c r="G274" s="1"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A275" s="7">
+        <v>275</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D275" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E275" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F275">
+        <v>12</v>
+      </c>
+      <c r="G275" s="1"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A276" s="7">
+        <v>276</v>
+      </c>
+      <c r="B276" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C276" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D276" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E276" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F276">
+        <v>12</v>
+      </c>
+      <c r="G276" s="1"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A277" s="7">
+        <v>277</v>
+      </c>
+      <c r="B277" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C277" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D277" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E277" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F277">
+        <v>12</v>
+      </c>
+      <c r="G277" s="1"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A278" s="7">
+        <v>278</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D278" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F278">
+        <v>12</v>
+      </c>
+      <c r="G278" s="1"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A279" s="7">
+        <v>279</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D279" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F279">
+        <v>13</v>
+      </c>
+      <c r="G279" s="1"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A280" s="7">
+        <v>280</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D280" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F280">
+        <v>12</v>
+      </c>
+      <c r="G280" s="1"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A281" s="7">
+        <v>281</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D281" s="9" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F281">
+        <v>13</v>
+      </c>
+      <c r="G281" s="1"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A282" s="7">
+        <v>282</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D282" s="9" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E282" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F282">
+        <v>13</v>
+      </c>
+      <c r="G282" s="1"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A283" s="7">
+        <v>283</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D283" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F283">
+        <v>13</v>
+      </c>
+      <c r="G283" s="1"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A284" s="7">
+        <v>284</v>
+      </c>
+      <c r="B284" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D284" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F284">
+        <v>11</v>
+      </c>
+      <c r="G284" s="1"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A285" s="7">
+        <v>285</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D285" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E285" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F285">
+        <v>11</v>
+      </c>
+      <c r="G285" s="1"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A286" s="7">
+        <v>286</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D286" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F286">
+        <v>11</v>
+      </c>
+      <c r="G286" s="1"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A287" s="7">
+        <v>287</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D287" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F287">
+        <v>11</v>
+      </c>
+      <c r="G287" s="1"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A288" s="7">
+        <v>288</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C288" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D288" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E288" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F288">
+        <v>11</v>
+      </c>
+      <c r="G288" s="1"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A289" s="7">
+        <v>289</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C289" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E289" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F289">
+        <v>11</v>
+      </c>
+      <c r="G289" s="1"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A290" s="7">
+        <v>290</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F290">
+        <v>11</v>
+      </c>
+      <c r="G290" s="1"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A291" s="7">
+        <v>291</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F291">
+        <v>11</v>
+      </c>
+      <c r="G291" s="1"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A292" s="7">
+        <v>292</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F292">
+        <v>11</v>
+      </c>
+      <c r="G292" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D273" r:id="rId1" display="https://pinci.ru/?utm_source=chatgpt.com"/>
+    <hyperlink ref="D281" r:id="rId2" display="https://2gis.ru/n_novgorod/search/%D0%9A%D0%BE%D0%BD%D0%B4%D0%B8%D1%82%D0%B5%D1%80%D1%81%D0%BA%D0%B8%D0%B5 %D0%B8%D0%B7%D0%B4%D0%B5%D0%BB%D0%B8%D1%8F/rubricId/363?utm_source=chatgpt.com"/>
+    <hyperlink ref="D282" r:id="rId3" display="https://yandex.ru/maps/org/mister_bublik/111013376298/?utm_source=chatgpt.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>